<commit_message>
updated files and webapp
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/ctrl-settings/eoseuwgdpir/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\NM\ctrl-settings\EoSEUwGDPiR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACA362D-1279-3C45-943D-FADD21733142}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83E42982-7CC6-4023-BFB5-749F7B18E190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10280" yWindow="1720" windowWidth="18520" windowHeight="14040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="765" windowWidth="26355" windowHeight="16020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="337">
   <si>
     <t>About</t>
   </si>
@@ -1047,6 +1047,9 @@
   </si>
   <si>
     <t>Tables 5a, 6, 7a, and 9a</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
   </si>
 </sst>
 </file>
@@ -1461,23 +1464,26 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B1" t="s">
+        <v>336</v>
+      </c>
       <c r="C1" s="26">
-        <v>44307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>44384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -1485,154 +1491,154 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B30"/>
     </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>329</v>
       </c>
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>330</v>
       </c>
       <c r="B32"/>
     </row>
-    <row r="33" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>328</v>
       </c>
@@ -1653,29 +1659,29 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="87.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>331</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>321</v>
       </c>
@@ -1683,12 +1689,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
@@ -1698,10 +1704,10 @@
       </c>
       <c r="C4">
         <f>EIA!D5</f>
-        <v>-2.748414376321353E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>-2.5423728813559324E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>57</v>
       </c>
@@ -1711,10 +1717,10 @@
       </c>
       <c r="C5">
         <f>EIA!I5</f>
-        <v>-6.7383216205043506E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>-6.892282294676029E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>56</v>
       </c>
@@ -1727,12 +1733,12 @@
         <v>-0.10839160839160844</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
@@ -1742,10 +1748,10 @@
       </c>
       <c r="C9">
         <f>EIA!D3</f>
-        <v>2.3093072078376489E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2.3809523809523808E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>57</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>56</v>
       </c>
@@ -1766,15 +1772,15 @@
       </c>
       <c r="C11">
         <f>EIA!I3</f>
-        <v>-7.7705156136528702E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>-8.0376538740043538E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>5</v>
       </c>
@@ -1784,10 +1790,10 @@
       </c>
       <c r="C14">
         <f>EIA!D4</f>
-        <v>-5.830258302583026E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>-5.6910569105691054E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>57</v>
       </c>
@@ -1799,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>56</v>
       </c>
@@ -1809,21 +1815,21 @@
       </c>
       <c r="C16">
         <f>EIA!I4</f>
-        <v>-9.0909090909091023E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-9.2827004219409356E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="23"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2019</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>29</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>18423</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>-(1-C20/B20)</f>
         <v>-5.2704648292883571E-2</v>
@@ -1854,12 +1860,12 @@
       </c>
       <c r="C22" s="15"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>7</v>
       </c>
@@ -1879,21 +1885,21 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="6">
         <f>SUMPRODUCT(B9:B11,C9:C11)/SUM(B9:B11)</f>
-        <v>-2.8811645571659744E-2</v>
+        <v>-2.9839714430803268E-2</v>
       </c>
       <c r="C26" s="6">
         <f>SUMPRODUCT(B14:B16,C14:C16)/SUM(B14:B16)</f>
-        <v>-7.2226829255599492E-2</v>
+        <v>-7.2267902842862455E-2</v>
       </c>
       <c r="D26" s="6">
         <f>SUMPRODUCT(B4:B6,C4:C6)/SUM(B4:B6)</f>
-        <v>-8.9350372675404757E-2</v>
+        <v>-8.9036114252317167E-2</v>
       </c>
       <c r="E26" s="6">
         <f>(EIA!C10-EIA!B10)/EIA!B10</f>
@@ -1901,29 +1907,29 @@
       </c>
       <c r="F26" s="13">
         <f>(EIA!C6-EIA!B6)/EIA!B6</f>
-        <v>-2.084942084942085E-2</v>
+        <v>-1.7986577181208052E-2</v>
       </c>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F27" s="12"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="11">
         <f>B26/$A$22</f>
-        <v>0.54666232495379397</v>
+        <v>0.5661685524392801</v>
       </c>
       <c r="C28" s="11">
         <f>C26/$A$22</f>
-        <v>1.3704071954759993</v>
+        <v>1.3711865116955995</v>
       </c>
       <c r="D28" s="11">
         <f>D26/$A$22</f>
-        <v>1.6953034612597777</v>
+        <v>1.689340829247868</v>
       </c>
       <c r="E28" s="11">
         <f>E26/$A$22</f>
@@ -1931,7 +1937,7 @@
       </c>
       <c r="F28" s="11">
         <f>F26/$A$22</f>
-        <v>0.39558979188247495</v>
+        <v>0.34127117367817983</v>
       </c>
       <c r="G28" s="14"/>
     </row>
@@ -1947,12 +1953,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>61</v>
       </c>
@@ -2154,7 +2160,7 @@
         <v>421200000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>62</v>
       </c>
@@ -2255,7 +2261,7 @@
         <v>1069000000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -2356,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>64</v>
       </c>
@@ -2457,7 +2463,7 @@
         <v>147800000000000</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>65</v>
       </c>
@@ -2558,7 +2564,7 @@
         <v>1153000000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>66</v>
       </c>
@@ -2659,7 +2665,7 @@
         <v>1963000000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2760,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2861,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -3063,7 +3069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -3265,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>73</v>
       </c>
@@ -3366,7 +3372,7 @@
         <v>2494000000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>74</v>
       </c>
@@ -3467,7 +3473,7 @@
         <v>44000000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -3568,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -3669,7 +3675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>77</v>
       </c>
@@ -3770,7 +3776,7 @@
         <v>1082000000000000</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>78</v>
       </c>
@@ -3871,7 +3877,7 @@
         <v>162800000000000</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>79</v>
       </c>
@@ -3972,7 +3978,7 @@
         <v>151900000000000</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -4073,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -4174,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -4275,7 +4281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>83</v>
       </c>
@@ -4376,7 +4382,7 @@
         <v>18570000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>84</v>
       </c>
@@ -4477,7 +4483,7 @@
         <v>5059000000000</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -4578,7 +4584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -4780,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>88</v>
       </c>
@@ -4881,7 +4887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -4982,7 +4988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -5083,7 +5089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>91</v>
       </c>
@@ -5184,7 +5190,7 @@
         <v>244300000000000</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -5285,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -5386,7 +5392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -5487,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -5588,7 +5594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -5689,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -5790,7 +5796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -5891,7 +5897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -5992,7 +5998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -6093,7 +6099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -6194,7 +6200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>102</v>
       </c>
@@ -6295,7 +6301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -6396,7 +6402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -6497,7 +6503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -6598,7 +6604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -6699,7 +6705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -6800,7 +6806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -6901,7 +6907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
         <v>109</v>
       </c>
@@ -7002,7 +7008,7 @@
         <v>151200000000000</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>110</v>
       </c>
@@ -7103,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -7204,7 +7210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -7305,7 +7311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
         <v>113</v>
       </c>
@@ -7406,7 +7412,7 @@
         <v>31710000000000</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>114</v>
       </c>
@@ -7507,7 +7513,7 @@
         <v>91150000000000</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -7608,7 +7614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>116</v>
       </c>
@@ -7709,7 +7715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>117</v>
       </c>
@@ -7810,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -7911,7 +7917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -8012,7 +8018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -8113,7 +8119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>121</v>
       </c>
@@ -8214,7 +8220,7 @@
         <v>104500000000000</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="s">
         <v>122</v>
       </c>
@@ -8315,7 +8321,7 @@
         <v>265200000000000</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -8416,7 +8422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" s="22" t="s">
         <v>124</v>
       </c>
@@ -8517,7 +8523,7 @@
         <v>36670000000000</v>
       </c>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>125</v>
       </c>
@@ -8618,7 +8624,7 @@
         <v>286000000000000</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67" s="22" t="s">
         <v>126</v>
       </c>
@@ -8719,7 +8725,7 @@
         <v>487200000000000</v>
       </c>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>127</v>
       </c>
@@ -8820,7 +8826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -8921,7 +8927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>129</v>
       </c>
@@ -9022,7 +9028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>130</v>
       </c>
@@ -9123,7 +9129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>131</v>
       </c>
@@ -9224,7 +9230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>132</v>
       </c>
@@ -9325,7 +9331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
         <v>133</v>
       </c>
@@ -9426,7 +9432,7 @@
         <v>618900000000000</v>
       </c>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" s="22" t="s">
         <v>134</v>
       </c>
@@ -9527,7 +9533,7 @@
         <v>10920000000000</v>
       </c>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>135</v>
       </c>
@@ -9628,7 +9634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -9729,7 +9735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" s="22" t="s">
         <v>137</v>
       </c>
@@ -9830,7 +9836,7 @@
         <v>268400000000000</v>
       </c>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="22" t="s">
         <v>138</v>
       </c>
@@ -9931,7 +9937,7 @@
         <v>40390000000000</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" s="22" t="s">
         <v>139</v>
       </c>
@@ -10032,7 +10038,7 @@
         <v>37700000000000</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>140</v>
       </c>
@@ -10133,7 +10139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>141</v>
       </c>
@@ -10234,7 +10240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>142</v>
       </c>
@@ -10335,7 +10341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A84" s="22" t="s">
         <v>143</v>
       </c>
@@ -10436,7 +10442,7 @@
         <v>4609000000000</v>
       </c>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85" s="22" t="s">
         <v>144</v>
       </c>
@@ -10537,7 +10543,7 @@
         <v>1256000000000</v>
       </c>
     </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>145</v>
       </c>
@@ -10638,7 +10644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>146</v>
       </c>
@@ -10739,7 +10745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>147</v>
       </c>
@@ -10840,7 +10846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>148</v>
       </c>
@@ -10941,7 +10947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>149</v>
       </c>
@@ -11042,7 +11048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>150</v>
       </c>
@@ -11143,7 +11149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92" s="22" t="s">
         <v>151</v>
       </c>
@@ -11244,7 +11250,7 @@
         <v>60630000000000</v>
       </c>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>152</v>
       </c>
@@ -11345,7 +11351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -11446,7 +11452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>154</v>
       </c>
@@ -11547,7 +11553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>155</v>
       </c>
@@ -11648,7 +11654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>156</v>
       </c>
@@ -11749,7 +11755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>157</v>
       </c>
@@ -11850,7 +11856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>158</v>
       </c>
@@ -11951,7 +11957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>159</v>
       </c>
@@ -12052,7 +12058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>160</v>
       </c>
@@ -12153,7 +12159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>161</v>
       </c>
@@ -12254,7 +12260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>162</v>
       </c>
@@ -12355,7 +12361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>163</v>
       </c>
@@ -12456,7 +12462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>164</v>
       </c>
@@ -12557,7 +12563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>165</v>
       </c>
@@ -12658,7 +12664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>166</v>
       </c>
@@ -12759,7 +12765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>167</v>
       </c>
@@ -12860,7 +12866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>168</v>
       </c>
@@ -12961,7 +12967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A110" s="22" t="s">
         <v>169</v>
       </c>
@@ -13062,7 +13068,7 @@
         <v>37530000000000</v>
       </c>
     </row>
-    <row r="111" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>170</v>
       </c>
@@ -13163,7 +13169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>171</v>
       </c>
@@ -13264,7 +13270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>172</v>
       </c>
@@ -13365,7 +13371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A114" s="22" t="s">
         <v>173</v>
       </c>
@@ -13466,7 +13472,7 @@
         <v>7869000000000</v>
       </c>
     </row>
-    <row r="115" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A115" s="22" t="s">
         <v>174</v>
       </c>
@@ -13567,7 +13573,7 @@
         <v>22620000000000</v>
       </c>
     </row>
-    <row r="116" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>175</v>
       </c>
@@ -13668,7 +13674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>176</v>
       </c>
@@ -13769,7 +13775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>177</v>
       </c>
@@ -13870,7 +13876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>178</v>
       </c>
@@ -13971,7 +13977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>179</v>
       </c>
@@ -14072,7 +14078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>180</v>
       </c>
@@ -14173,7 +14179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A122" s="22" t="s">
         <v>181</v>
       </c>
@@ -14274,7 +14280,7 @@
         <v>88660000000000</v>
       </c>
     </row>
-    <row r="123" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A123" s="22" t="s">
         <v>182</v>
       </c>
@@ -14375,7 +14381,7 @@
         <v>1045000000000000</v>
       </c>
     </row>
-    <row r="124" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>183</v>
       </c>
@@ -14476,7 +14482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A125" s="22" t="s">
         <v>184</v>
       </c>
@@ -14577,7 +14583,7 @@
         <v>335000000000000</v>
       </c>
     </row>
-    <row r="126" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A126" s="22" t="s">
         <v>185</v>
       </c>
@@ -14678,7 +14684,7 @@
         <v>868000000000000</v>
       </c>
     </row>
-    <row r="127" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A127" s="22" t="s">
         <v>186</v>
       </c>
@@ -14779,7 +14785,7 @@
         <v>3561000000000000</v>
       </c>
     </row>
-    <row r="128" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>187</v>
       </c>
@@ -14880,7 +14886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>188</v>
       </c>
@@ -14981,7 +14987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>189</v>
       </c>
@@ -15082,7 +15088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>190</v>
       </c>
@@ -15183,7 +15189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>191</v>
       </c>
@@ -15284,7 +15290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A133" s="22" t="s">
         <v>192</v>
       </c>
@@ -15385,7 +15391,7 @@
         <v>24420000000000</v>
       </c>
     </row>
-    <row r="134" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A134" s="22" t="s">
         <v>193</v>
       </c>
@@ -15486,7 +15492,7 @@
         <v>1828000000000000</v>
       </c>
     </row>
-    <row r="135" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A135" s="22" t="s">
         <v>194</v>
       </c>
@@ -15587,7 +15593,7 @@
         <v>23090000000000</v>
       </c>
     </row>
-    <row r="136" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>195</v>
       </c>
@@ -15688,7 +15694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>196</v>
       </c>
@@ -15789,7 +15795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A138" s="22" t="s">
         <v>197</v>
       </c>
@@ -15890,7 +15896,7 @@
         <v>1258000000000000</v>
       </c>
     </row>
-    <row r="139" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A139" s="22" t="s">
         <v>198</v>
       </c>
@@ -15991,7 +15997,7 @@
         <v>777700000000000</v>
       </c>
     </row>
-    <row r="140" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A140" s="22" t="s">
         <v>199</v>
       </c>
@@ -16092,7 +16098,7 @@
         <v>163200000000000</v>
       </c>
     </row>
-    <row r="141" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>200</v>
       </c>
@@ -16193,7 +16199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>201</v>
       </c>
@@ -16294,7 +16300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>202</v>
       </c>
@@ -16395,7 +16401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A144" s="22" t="s">
         <v>203</v>
       </c>
@@ -16496,7 +16502,7 @@
         <v>5642000000000</v>
       </c>
     </row>
-    <row r="145" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A145" s="22" t="s">
         <v>204</v>
       </c>
@@ -16597,7 +16603,7 @@
         <v>116500000000000</v>
       </c>
     </row>
-    <row r="146" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A146" s="22" t="s">
         <v>205</v>
       </c>
@@ -16698,7 +16704,7 @@
         <v>313500000000000</v>
       </c>
     </row>
-    <row r="147" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>206</v>
       </c>
@@ -16799,7 +16805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>207</v>
       </c>
@@ -16900,7 +16906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>208</v>
       </c>
@@ -17001,7 +17007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>209</v>
       </c>
@@ -17102,7 +17108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>210</v>
       </c>
@@ -17203,7 +17209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>211</v>
       </c>
@@ -17304,7 +17310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>212</v>
       </c>
@@ -17405,7 +17411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>213</v>
       </c>
@@ -17506,7 +17512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>214</v>
       </c>
@@ -17607,7 +17613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>215</v>
       </c>
@@ -17708,7 +17714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>216</v>
       </c>
@@ -17809,7 +17815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>217</v>
       </c>
@@ -17910,7 +17916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>218</v>
       </c>
@@ -18011,7 +18017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>219</v>
       </c>
@@ -18112,7 +18118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>220</v>
       </c>
@@ -18213,7 +18219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>221</v>
       </c>
@@ -18314,7 +18320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>222</v>
       </c>
@@ -18415,7 +18421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>223</v>
       </c>
@@ -18516,7 +18522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>224</v>
       </c>
@@ -18617,7 +18623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>225</v>
       </c>
@@ -18718,7 +18724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>226</v>
       </c>
@@ -18819,7 +18825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>227</v>
       </c>
@@ -18920,7 +18926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>228</v>
       </c>
@@ -19021,7 +19027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A170" s="22" t="s">
         <v>229</v>
       </c>
@@ -19122,7 +19128,7 @@
         <v>335300000000000</v>
       </c>
     </row>
-    <row r="171" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>230</v>
       </c>
@@ -19223,7 +19229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>231</v>
       </c>
@@ -19324,7 +19330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>232</v>
       </c>
@@ -19425,7 +19431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A174" s="22" t="s">
         <v>233</v>
       </c>
@@ -19526,7 +19532,7 @@
         <v>11590000000000</v>
       </c>
     </row>
-    <row r="175" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A175" s="22" t="s">
         <v>234</v>
       </c>
@@ -19627,7 +19633,7 @@
         <v>239300000000000</v>
       </c>
     </row>
-    <row r="176" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>235</v>
       </c>
@@ -19728,7 +19734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>236</v>
       </c>
@@ -19829,7 +19835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>237</v>
       </c>
@@ -19930,7 +19936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>238</v>
       </c>
@@ -20031,7 +20037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>239</v>
       </c>
@@ -20132,7 +20138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>240</v>
       </c>
@@ -20244,9 +20250,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -20347,7 +20353,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>241</v>
       </c>
@@ -20448,7 +20454,7 @@
         <v>43400000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>242</v>
       </c>
@@ -20549,7 +20555,7 @@
         <v>106900000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>243</v>
       </c>
@@ -20650,7 +20656,7 @@
         <v>47200000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -20751,7 +20757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>245</v>
       </c>
@@ -20852,7 +20858,7 @@
         <v>48300000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>246</v>
       </c>
@@ -20953,7 +20959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>247</v>
       </c>
@@ -21054,7 +21060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>248</v>
       </c>
@@ -21155,7 +21161,7 @@
         <v>14500000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>249</v>
       </c>
@@ -21256,7 +21262,7 @@
         <v>200000000000</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>250</v>
       </c>
@@ -21357,7 +21363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>251</v>
       </c>
@@ -21458,7 +21464,7 @@
         <v>196500000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>252</v>
       </c>
@@ -21559,7 +21565,7 @@
         <v>32600000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>253</v>
       </c>
@@ -21660,7 +21666,7 @@
         <v>5321000000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>254</v>
       </c>
@@ -21761,7 +21767,7 @@
         <v>932100000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>255</v>
       </c>
@@ -21862,7 +21868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>256</v>
       </c>
@@ -21963,7 +21969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>257</v>
       </c>
@@ -22064,7 +22070,7 @@
         <v>3.94654E+16</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>258</v>
       </c>
@@ -22165,7 +22171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>259</v>
       </c>
@@ -22266,7 +22272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>260</v>
       </c>
@@ -22367,7 +22373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>261</v>
       </c>
@@ -22468,7 +22474,7 @@
         <v>203800000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>262</v>
       </c>
@@ -22569,7 +22575,7 @@
         <v>471400000000000</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>263</v>
       </c>
@@ -22670,7 +22676,7 @@
         <v>372200000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>264</v>
       </c>
@@ -22771,7 +22777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>265</v>
       </c>
@@ -22872,7 +22878,7 @@
         <v>1500000000000</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>266</v>
       </c>
@@ -22973,7 +22979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>267</v>
       </c>
@@ -23074,7 +23080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>268</v>
       </c>
@@ -23175,7 +23181,7 @@
         <v>23500000000000</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>269</v>
       </c>
@@ -23276,7 +23282,7 @@
         <v>100000000000</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>270</v>
       </c>
@@ -23377,7 +23383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>271</v>
       </c>
@@ -23478,7 +23484,7 @@
         <v>509100000000000</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>272</v>
       </c>
@@ -23579,7 +23585,7 @@
         <v>56200000000000</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>273</v>
       </c>
@@ -23680,7 +23686,7 @@
         <v>5621000000000000</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>274</v>
       </c>
@@ -23781,7 +23787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>275</v>
       </c>
@@ -23882,7 +23888,7 @@
         <v>132300000000000</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>276</v>
       </c>
@@ -23983,7 +23989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>277</v>
       </c>
@@ -24084,7 +24090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>278</v>
       </c>
@@ -24185,7 +24191,7 @@
         <v>156300000000000</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>279</v>
       </c>
@@ -24286,7 +24292,7 @@
         <v>6015600000000000</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>280</v>
       </c>
@@ -24387,7 +24393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>281</v>
       </c>
@@ -24488,7 +24494,7 @@
         <v>84010000000000</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>282</v>
       </c>
@@ -24589,7 +24595,7 @@
         <v>98200000000000</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>283</v>
       </c>
@@ -24690,7 +24696,7 @@
         <v>70220000000000</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>284</v>
       </c>
@@ -24791,7 +24797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>285</v>
       </c>
@@ -24892,7 +24898,7 @@
         <v>45450000000000</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>286</v>
       </c>
@@ -24993,7 +24999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>287</v>
       </c>
@@ -25094,7 +25100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>288</v>
       </c>
@@ -25195,7 +25201,7 @@
         <v>15807100000000</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>289</v>
       </c>
@@ -25296,7 +25302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>290</v>
       </c>
@@ -25397,7 +25403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
         <v>291</v>
       </c>
@@ -25498,7 +25504,7 @@
         <v>263000000000000</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>292</v>
       </c>
@@ -25599,7 +25605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>293</v>
       </c>
@@ -25700,7 +25706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>294</v>
       </c>
@@ -25801,7 +25807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>295</v>
       </c>
@@ -25902,7 +25908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>296</v>
       </c>
@@ -26003,7 +26009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>297</v>
       </c>
@@ -26104,7 +26110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>298</v>
       </c>
@@ -26205,7 +26211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>299</v>
       </c>
@@ -26306,7 +26312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>300</v>
       </c>
@@ -26407,7 +26413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>301</v>
       </c>
@@ -26508,7 +26514,7 @@
         <v>355700000000000</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>302</v>
       </c>
@@ -26609,7 +26615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" s="22" t="s">
         <v>303</v>
       </c>
@@ -26710,7 +26716,7 @@
         <v>218800000000000</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>304</v>
       </c>
@@ -26811,7 +26817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>305</v>
       </c>
@@ -26912,7 +26918,7 @@
         <v>693000000000000</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>306</v>
       </c>
@@ -27013,7 +27019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>307</v>
       </c>
@@ -27114,7 +27120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69" s="22" t="s">
         <v>308</v>
       </c>
@@ -27215,7 +27221,7 @@
         <v>94200000000000</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="s">
         <v>309</v>
       </c>
@@ -27316,7 +27322,7 @@
         <v>113500000000000</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>310</v>
       </c>
@@ -27417,7 +27423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" s="22" t="s">
         <v>311</v>
       </c>
@@ -27518,7 +27524,7 @@
         <v>2392000000000000</v>
       </c>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
         <v>312</v>
       </c>
@@ -27619,7 +27625,7 @@
         <v>167300000000000</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
         <v>313</v>
       </c>
@@ -27720,7 +27726,7 @@
         <v>3816000000000000</v>
       </c>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>314</v>
       </c>
@@ -27821,7 +27827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" s="22" t="s">
         <v>315</v>
       </c>
@@ -27922,7 +27928,7 @@
         <v>2975000000000000</v>
       </c>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>316</v>
       </c>
@@ -28023,7 +28029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>317</v>
       </c>
@@ -28124,7 +28130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="22" t="s">
         <v>318</v>
       </c>
@@ -28225,7 +28231,7 @@
         <v>241162000000000</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" s="22" t="s">
         <v>319</v>
       </c>
@@ -28326,7 +28332,7 @@
         <v>120600000000000</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>320</v>
       </c>
@@ -28437,16 +28443,16 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
@@ -28460,7 +28466,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>322</v>
       </c>
@@ -28486,106 +28492,108 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="C3">
         <v>1462</v>
       </c>
       <c r="D3">
         <f>(C3-B3)/B3</f>
-        <v>2.3093072078376489E-2</v>
+        <v>2.3809523809523808E-2</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
       </c>
       <c r="G3">
-        <v>13.77</v>
+        <v>13.81</v>
       </c>
       <c r="H3">
         <v>12.7</v>
       </c>
       <c r="I3">
         <f>(H3-G3)/G3</f>
-        <v>-7.7705156136528702E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-8.0376538740043538E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="C4">
         <v>1276</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D6" si="0">(C4-B4)/B4</f>
-        <v>-5.830258302583026E-2</v>
+        <v>-5.6910569105691054E-2</v>
       </c>
       <c r="F4" t="s">
         <v>35</v>
       </c>
       <c r="G4">
-        <v>9.4600000000000009</v>
+        <v>9.48</v>
       </c>
       <c r="H4">
         <v>8.6</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I5" si="1">(H4-G4)/G4</f>
-        <v>-9.0909090909091023E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-9.2827004219409356E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="B5">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C5">
         <v>920</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>-2.748414376321353E-2</v>
+        <v>-2.5423728813559324E-2</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
       </c>
       <c r="G5">
-        <v>24.19</v>
+        <v>24.23</v>
       </c>
       <c r="H5">
         <v>22.56</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>-6.7383216205043506E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-6.892282294676029E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
       <c r="B6">
-        <v>3885</v>
+        <f>SUM(B3:B5)</f>
+        <v>3725</v>
       </c>
       <c r="C6">
-        <v>3804</v>
+        <f>SUM(C3:C5)</f>
+        <v>3658</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-2.084942084942085E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-1.7986577181208052E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -28599,7 +28607,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>43</v>
       </c>
@@ -28622,7 +28630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>31</v>
       </c>
@@ -28650,7 +28658,7 @@
         <v>0.14285714285714299</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>55</v>
       </c>
@@ -28665,7 +28673,7 @@
         <v>-0.10839160839160844</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -28692,14 +28700,16 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -28707,7 +28717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -28716,43 +28726,43 @@
         <v>2.7024046102025086</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="14">
         <f>Calculations!F28</f>
-        <v>0.39558979188247495</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.34127117367817983</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="7">
         <f>Calculations!B28</f>
-        <v>0.54666232495379397</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.5661685524392801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="7">
         <f>Calculations!C28</f>
-        <v>1.3704071954759993</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1.3711865116955995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="7">
         <f>Calculations!D28</f>
-        <v>1.6953034612597777</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1.689340829247868</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -28760,7 +28770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -28768,7 +28778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>